<commit_message>
Changes and fixes to read multiple row data
</commit_message>
<xml_diff>
--- a/PHPTravels/src/com/php/resources/PhpTravelsBookingData.xlsx
+++ b/PHPTravels/src/com/php/resources/PhpTravelsBookingData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Workspace\PHPTravels\src\com\php\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devik\git\Sep2020\PHPTravels\src\com\php\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6A9F8A-8896-4C21-8E9F-0902FF56CC4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEA6BD3-5353-4A7C-B588-4B50ACB776B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{854A6EE8-0253-49AA-8564-C3F90A48F51B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Mumbai</t>
+  </si>
+  <si>
+    <t>Book2Children</t>
+  </si>
+  <si>
+    <t>Chennai</t>
   </si>
 </sst>
 </file>
@@ -414,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C39C44-7F4A-4E60-8D19-D8DFFB0CCB53}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,6 +475,20 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>